<commit_message>
Add register action in that-lan-von-cau
</commit_message>
<xml_diff>
--- a/kwfinder.xlsx
+++ b/kwfinder.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15000" windowHeight="7380" tabRatio="777" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15000" windowHeight="7380" tabRatio="813" firstSheet="3" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Giới thiệu" sheetId="2" r:id="rId1"/>
@@ -20,13 +20,15 @@
     <sheet name="Tứ quý" sheetId="6" r:id="rId6"/>
     <sheet name="Tượng" sheetId="7" r:id="rId7"/>
     <sheet name="Thất lân" sheetId="8" r:id="rId8"/>
+    <sheet name="Chuông" sheetId="9" r:id="rId9"/>
+    <sheet name="Ngũ sự" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="160">
   <si>
     <t>đồ đồng</t>
   </si>
@@ -479,6 +481,33 @@
   </si>
   <si>
     <t>601</t>
+  </si>
+  <si>
+    <t>chuông đồng</t>
+  </si>
+  <si>
+    <t>đồng đỏ</t>
+  </si>
+  <si>
+    <t>đồng vàng</t>
+  </si>
+  <si>
+    <t>162,000 </t>
+  </si>
+  <si>
+    <t>13,600 </t>
+  </si>
+  <si>
+    <t>5,290 </t>
+  </si>
+  <si>
+    <t>320 </t>
+  </si>
+  <si>
+    <t>bộ đỉnh đồng ngũ sự</t>
+  </si>
+  <si>
+    <t>bộ đỉnh ngũ sự</t>
   </si>
 </sst>
 </file>
@@ -576,7 +605,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -639,6 +668,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -991,12 +1021,66 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.625" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.625" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="15"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" s="14">
+        <v>70</v>
+      </c>
+      <c r="C2" s="14">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="B3" s="15">
+        <v>10</v>
+      </c>
+      <c r="C3" s="15">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1313,7 +1397,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1443,7 +1527,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1580,8 +1664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1809,10 +1893,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1822,7 +1906,7 @@
     <col min="3" max="3" width="11.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>68</v>
       </c>
@@ -1832,8 +1916,14 @@
       <c r="C1" s="11" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>129</v>
       </c>
@@ -1843,8 +1933,15 @@
       <c r="C2" s="12" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" s="28" t="s">
+        <v>154</v>
+      </c>
+      <c r="E2" s="15" t="str">
+        <f>CONCATENATE("intitle:",CHAR(34),A2,CHAR(34))</f>
+        <v>intitle:"tứ quý"</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>89</v>
       </c>
@@ -1854,8 +1951,12 @@
       <c r="C3" s="12" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E3" s="15" t="str">
+        <f>CONCATENATE("intitle:",CHAR(34),A3,CHAR(34))</f>
+        <v>intitle:"tranh tu quy"</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
         <v>128</v>
       </c>
@@ -1865,8 +1966,12 @@
       <c r="C4" s="12" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E4" s="15" t="str">
+        <f t="shared" ref="E4:E10" si="0">CONCATENATE("intitle:",CHAR(34),A4,CHAR(34))</f>
+        <v>intitle:"sim tứ quý giá rẻ"</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>125</v>
       </c>
@@ -1876,8 +1981,15 @@
       <c r="C5" s="12" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="E5" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>intitle:"tranh tứ quý"</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>124</v>
       </c>
@@ -1887,8 +1999,12 @@
       <c r="C6" s="12" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E6" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>intitle:"tu quy"</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>123</v>
       </c>
@@ -1898,8 +2014,12 @@
       <c r="C7" s="12" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E7" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>intitle:"bộ tranh tứ quý"</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>122</v>
       </c>
@@ -1909,8 +2029,15 @@
       <c r="C8" s="12" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8" s="28" t="s">
+        <v>157</v>
+      </c>
+      <c r="E8" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>intitle:"tranh tùng cúc trúc mai"</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>120</v>
       </c>
@@ -1920,8 +2047,15 @@
       <c r="C9" s="12" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="E9" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>intitle:"tùng cúc trúc mai"</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
         <v>117</v>
       </c>
@@ -1931,6 +2065,19 @@
       <c r="C10" s="12" t="s">
         <v>18</v>
       </c>
+      <c r="E10" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>intitle:"cach treo tranh tu quy"</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E11" s="15"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E12" s="15"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E13" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1941,8 +2088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1983,8 +2130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2031,4 +2178,70 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.625" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.625" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="15"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="B2" s="14">
+        <v>420</v>
+      </c>
+      <c r="C2" s="14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="B3" s="15">
+        <v>710</v>
+      </c>
+      <c r="C3" s="15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="B4" s="15">
+        <v>460</v>
+      </c>
+      <c r="C4" s="15">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
re-organize folder landing pages
</commit_message>
<xml_diff>
--- a/kwfinder.xlsx
+++ b/kwfinder.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15000" windowHeight="7380" tabRatio="813" firstSheet="3" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15000" windowHeight="7380" tabRatio="813"/>
   </bookViews>
   <sheets>
     <sheet name="Giới thiệu" sheetId="2" r:id="rId1"/>
@@ -605,7 +605,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -669,6 +669,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -951,7 +952,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -1025,7 +1026,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -1665,7 +1666,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1881,13 +1882,17 @@
       <c r="C13" s="12" t="s">
         <v>13</v>
       </c>
+      <c r="D13" s="29">
+        <v>1190</v>
+      </c>
       <c r="E13" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("intitle:",CHAR(34),A13,CHAR(34))</f>
         <v>intitle:"trống đồng ngọc lũ"</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>